<commit_message>
Add Chance Column Create Battle Hierarchy and order
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Resources/Documents/ComplexAbilities/ComplexAbililties.xlsx
+++ b/Assets/Scripts/1.Abilities/Resources/Documents/ComplexAbilities/ComplexAbililties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Resources\Documents\ComplexAbilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Resources\Documents\ComplexAbilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77C602-71B8-4AA8-929B-C20F32C24F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6848F8A8-9E23-4F71-9BAD-4100C62DDFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="28800" windowHeight="15345" firstSheet="3" activeTab="4" xr2:uid="{43129CA1-51D5-4C92-9A38-1A83E66F1476}"/>
+    <workbookView xWindow="7460" yWindow="2610" windowWidth="28800" windowHeight="15460" xr2:uid="{43129CA1-51D5-4C92-9A38-1A83E66F1476}"/>
   </bookViews>
   <sheets>
     <sheet name="AreaDurationAimedAbility" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="11">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,10 @@
   </si>
   <si>
     <t>Motivation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -446,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B6C90D-190D-468E-AB43-27C4950A1E42}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,111 +477,114 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G2" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G3" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G5" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G6" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G7" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G8" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G9" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G10" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G11" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G12" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G14" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G15" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G16" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G17" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -586,15 +593,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55566779-8205-4BA0-BF7D-874EB067FF08}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,57 +623,60 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H3" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H4" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H5" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H6" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H7" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H8" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -675,15 +685,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C73EA9A-E9F9-4FA9-8405-43CACD580FDA}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,75 +709,78 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F11" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -776,15 +789,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF823A4-9422-4055-914D-921C5F34C1B4}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -806,105 +819,108 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H3" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H4" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H5" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H6" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H7" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H8" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H9" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H10" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H11" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H12" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H13" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H14" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H15" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H16" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,15 +929,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C6EC0B-DBD4-439E-A258-DBBA120310D1}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,57 +962,60 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I3" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I4" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I5" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I6" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I7" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I8" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1005,15 +1024,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C0A86A-8129-457F-91CA-19F416369FF2}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1032,99 +1051,102 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G2" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G3" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G5" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G6" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G7" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G8" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G9" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G10" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G11" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G12" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G14" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G15" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1133,15 +1155,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3A991-8850-48F2-9581-C4B3886CA4A3}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,105 +1179,108 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F11" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F12" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F13" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F14" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F15" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>